<commit_message>
navn for dag 1
</commit_message>
<xml_diff>
--- a/gutter.xlsx
+++ b/gutter.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28502"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28615"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anr/Dropbox/Documents/Torpa-IL/Synnfjell Arrangementer AS/resultat-maler/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anr/Dropbox/Documents/Torpa-IL/Synnfjell Arrangementer AS/TdS-2017/resultater/tds/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20460" tabRatio="991" activeTab="13"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33140" windowHeight="20460" tabRatio="991"/>
   </bookViews>
   <sheets>
     <sheet name="K1" sheetId="1" r:id="rId1"/>
@@ -161,7 +161,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="51">
   <si>
     <t>Dag1</t>
   </si>
@@ -272,6 +272,48 @@
   </si>
   <si>
     <t>Tour de Synnfjell Sammenlagt - Gutter 11-16</t>
+  </si>
+  <si>
+    <t>Jonatan Heimdal Korshavn</t>
+  </si>
+  <si>
+    <t>Marius Granvold</t>
+  </si>
+  <si>
+    <t>Magnus Moslett Evensen</t>
+  </si>
+  <si>
+    <t>Martin Jørstad Ringli</t>
+  </si>
+  <si>
+    <t>Eskil Engdal</t>
+  </si>
+  <si>
+    <t>Tobias Gigstad Bergene</t>
+  </si>
+  <si>
+    <t>Brage Sømoen</t>
+  </si>
+  <si>
+    <t>Jakob Lundby</t>
+  </si>
+  <si>
+    <t>Anders Alme Eng</t>
+  </si>
+  <si>
+    <t>Vegard Thon</t>
+  </si>
+  <si>
+    <t>Christian Thon Christensen</t>
+  </si>
+  <si>
+    <t>Per Ingvar Tollehaug</t>
+  </si>
+  <si>
+    <t>Hermann Byfuglien Ulsrud</t>
+  </si>
+  <si>
+    <t>Erland Andersen</t>
   </si>
 </sst>
 </file>
@@ -874,12 +916,13 @@
   <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:M104"/>
   <sheetViews>
-    <sheetView zoomScale="185" zoomScaleNormal="185" zoomScalePageLayoutView="185" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="185" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="26.33203125" customWidth="1"/>
     <col min="2" max="2" width="11.5" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="13" width="8.83203125" style="1"/>
   </cols>
@@ -965,33 +1008,35 @@
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" s="9"/>
+      <c r="A4" s="9" t="s">
+        <v>39</v>
+      </c>
       <c r="B4" s="25"/>
       <c r="C4" s="10" t="str">
         <f>IF(A4="","",IFERROR(RANK(B4,$B$4:$B$300,1),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="D4" s="11" t="str">
         <f>IF(A4="","", IFERROR(VLOOKUP(C4,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="E4" s="25"/>
       <c r="F4" s="10" t="str">
         <f>IF(A4="", "", IFERROR(RANK(E4,$E$4:$E$300,1),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="G4" s="11" t="str">
         <f>IF(A4="","",IFERROR(VLOOKUP(F4,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="H4" s="25"/>
       <c r="I4" s="10" t="str">
         <f>IF(A4="","",IFERROR(RANK(H4,$H$4:$H$300,1),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="J4" s="12" t="str">
         <f>IF(A4="","",IFERROR(VLOOKUP(I4,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="K4" s="26" t="str">
         <f>IF(A4="","",IFERROR(IF(B4+E4+H4=0,"",B4+E4+H4), "-"))</f>
@@ -999,41 +1044,43 @@
       </c>
       <c r="L4" s="10" t="str">
         <f>IF(A4="","",IFERROR(RANK(M4,$M$4:$M$300,0),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="M4" s="12" t="str">
         <f>IF(A4="","",IFERROR(IF(D4+G4+J4=0,"0",D4+G4+J4),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="9"/>
+      <c r="A5" s="9" t="s">
+        <v>37</v>
+      </c>
       <c r="B5" s="25"/>
       <c r="C5" s="10" t="str">
         <f t="shared" ref="C5:C68" si="0">IF(A5="","",IFERROR(RANK(B5,$B$4:$B$300,1),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="D5" s="11" t="str">
         <f>IF(A5="","", IFERROR(VLOOKUP(C5,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="E5" s="25"/>
       <c r="F5" s="10" t="str">
         <f t="shared" ref="F5:F68" si="1">IF(A5="", "", IFERROR(RANK(E5,$E$4:$E$300,1),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="G5" s="11" t="str">
         <f>IF(A5="","",IFERROR(VLOOKUP(F5,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="H5" s="25"/>
       <c r="I5" s="10" t="str">
         <f t="shared" ref="I5:I68" si="2">IF(A5="","",IFERROR(RANK(H5,$H$4:$H$300,1),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="J5" s="12" t="str">
         <f>IF(A5="","",IFERROR(VLOOKUP(I5,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="K5" s="26" t="str">
         <f t="shared" ref="K5:K68" si="3">IF(A5="","",IFERROR(IF(B5+E5+H5=0,"",B5+E5+H5), "-"))</f>
@@ -1041,41 +1088,43 @@
       </c>
       <c r="L5" s="10" t="str">
         <f t="shared" ref="L5:L68" si="4">IF(A5="","",IFERROR(RANK(M5,$M$4:$M$300,0),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="M5" s="12" t="str">
         <f t="shared" ref="M5:M68" si="5">IF(A5="","",IFERROR(IF(D5+G5+J5=0,"0",D5+G5+J5),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="9"/>
+      <c r="A6" s="9" t="s">
+        <v>40</v>
+      </c>
       <c r="B6" s="25"/>
       <c r="C6" s="10" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="D6" s="11" t="str">
         <f>IF(A6="","", IFERROR(VLOOKUP(C6,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="E6" s="25"/>
       <c r="F6" s="10" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="G6" s="11" t="str">
         <f>IF(A6="","",IFERROR(VLOOKUP(F6,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="H6" s="25"/>
       <c r="I6" s="10" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="J6" s="12" t="str">
         <f>IF(A6="","",IFERROR(VLOOKUP(I6,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="K6" s="26" t="str">
         <f t="shared" si="3"/>
@@ -1083,41 +1132,43 @@
       </c>
       <c r="L6" s="10" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="M6" s="12" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>-</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="9"/>
+      <c r="A7" s="9" t="s">
+        <v>38</v>
+      </c>
       <c r="B7" s="25"/>
       <c r="C7" s="10" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="D7" s="11" t="str">
         <f>IF(A7="","", IFERROR(VLOOKUP(C7,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="E7" s="25"/>
       <c r="F7" s="10" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="G7" s="11" t="str">
         <f>IF(A7="","",IFERROR(VLOOKUP(F7,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="H7" s="25"/>
       <c r="I7" s="10" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="J7" s="12" t="str">
         <f>IF(A7="","",IFERROR(VLOOKUP(I7,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="K7" s="26" t="str">
         <f t="shared" si="3"/>
@@ -1125,11 +1176,11 @@
       </c>
       <c r="L7" s="10" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="M7" s="12" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>-</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
@@ -5185,13 +5236,13 @@
   <sheetPr codeName="Sheet10" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:M103"/>
   <sheetViews>
-    <sheetView zoomScale="185" zoomScaleNormal="185" zoomScalePageLayoutView="185" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="185" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="33"/>
+    <col min="1" max="1" width="31.83203125" style="33" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.5" style="40" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.6640625" style="40" customWidth="1"/>
     <col min="4" max="13" width="8.83203125" style="40"/>
@@ -5253,15 +5304,15 @@
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="39" t="str">
         <f>IF('K3'!A4="", "",'K3'!A4)</f>
-        <v/>
-      </c>
-      <c r="B4" s="36" t="str">
+        <v>Brage Sømoen</v>
+      </c>
+      <c r="B4" s="36">
         <f>IF('K3'!A4="", "",'K3'!B4)</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="C4" s="37" t="str">
         <f>IF('K3'!A4="", "",'K3'!C4)</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="D4" s="35"/>
       <c r="E4" s="36"/>
@@ -5277,15 +5328,15 @@
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="39" t="str">
         <f>IF('K3'!A5="", "",'K3'!A5)</f>
-        <v/>
-      </c>
-      <c r="B5" s="36" t="str">
+        <v>Jakob Lundby</v>
+      </c>
+      <c r="B5" s="36">
         <f>IF('K3'!A5="", "",'K3'!B5)</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="C5" s="37" t="str">
         <f>IF('K3'!A5="", "",'K3'!C5)</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="D5" s="35"/>
       <c r="E5" s="36"/>
@@ -5301,15 +5352,15 @@
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="39" t="str">
         <f>IF('K3'!A6="", "",'K3'!A6)</f>
-        <v/>
-      </c>
-      <c r="B6" s="36" t="str">
+        <v>Anders Alme Eng</v>
+      </c>
+      <c r="B6" s="36">
         <f>IF('K3'!A6="", "",'K3'!B6)</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="C6" s="37" t="str">
         <f>IF('K3'!A6="", "",'K3'!C6)</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="D6" s="35"/>
       <c r="E6" s="36"/>
@@ -5325,15 +5376,15 @@
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="39" t="str">
         <f>IF('K3'!A7="", "",'K3'!A7)</f>
-        <v/>
-      </c>
-      <c r="B7" s="36" t="str">
+        <v>Vegard Thon</v>
+      </c>
+      <c r="B7" s="36">
         <f>IF('K3'!A7="", "",'K3'!B7)</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="C7" s="37" t="str">
         <f>IF('K3'!A7="", "",'K3'!C7)</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="D7" s="35"/>
       <c r="E7" s="36"/>
@@ -5349,15 +5400,15 @@
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="39" t="str">
         <f>IF('K3'!A8="", "",'K3'!A8)</f>
-        <v/>
-      </c>
-      <c r="B8" s="36" t="str">
+        <v>Christian Thon Christensen</v>
+      </c>
+      <c r="B8" s="36">
         <f>IF('K3'!A8="", "",'K3'!B8)</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="C8" s="37" t="str">
         <f>IF('K3'!A8="", "",'K3'!C8)</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="D8" s="35"/>
       <c r="E8" s="36"/>
@@ -5373,15 +5424,15 @@
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="39" t="str">
         <f>IF('K3'!A9="", "",'K3'!A9)</f>
-        <v/>
-      </c>
-      <c r="B9" s="36" t="str">
+        <v>Per Ingvar Tollehaug</v>
+      </c>
+      <c r="B9" s="36">
         <f>IF('K3'!A9="", "",'K3'!B9)</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="C9" s="37" t="str">
         <f>IF('K3'!A9="", "",'K3'!C9)</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="D9" s="35"/>
       <c r="E9" s="36"/>
@@ -5397,15 +5448,15 @@
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="39" t="str">
         <f>IF('K3'!A10="", "",'K3'!A10)</f>
-        <v/>
-      </c>
-      <c r="B10" s="36" t="str">
+        <v>Hermann Byfuglien Ulsrud</v>
+      </c>
+      <c r="B10" s="36">
         <f>IF('K3'!A10="", "",'K3'!B10)</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="C10" s="37" t="str">
         <f>IF('K3'!A10="", "",'K3'!C10)</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="D10" s="35"/>
       <c r="E10" s="36"/>
@@ -5421,15 +5472,15 @@
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="39" t="str">
         <f>IF('K3'!A11="", "",'K3'!A11)</f>
-        <v/>
-      </c>
-      <c r="B11" s="36" t="str">
+        <v>Erland Andersen</v>
+      </c>
+      <c r="B11" s="36">
         <f>IF('K3'!A11="", "",'K3'!B11)</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="C11" s="37" t="str">
         <f>IF('K3'!A11="", "",'K3'!C11)</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="D11" s="35"/>
       <c r="E11" s="36"/>
@@ -7644,13 +7695,13 @@
   <sheetPr codeName="Sheet11" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:M103"/>
   <sheetViews>
-    <sheetView zoomScale="185" zoomScaleNormal="185" zoomScalePageLayoutView="185" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="185" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="15"/>
+    <col min="1" max="1" width="31.83203125" style="15" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.5" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.6640625" style="1" customWidth="1"/>
     <col min="4" max="13" width="8.83203125" style="1"/>
@@ -7712,15 +7763,15 @@
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="str">
         <f>IF('K3'!A4="", "",'K3'!A4)</f>
-        <v/>
-      </c>
-      <c r="B4" s="25" t="str">
+        <v>Brage Sømoen</v>
+      </c>
+      <c r="B4" s="25">
         <f>IF('K3'!A4="", "",'K3'!E4)</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="C4" s="37" t="str">
         <f>IF('K3'!A4="", "",'K3'!F4)</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="D4" s="35"/>
       <c r="E4" s="25"/>
@@ -7736,15 +7787,15 @@
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="str">
         <f>IF('K3'!A5="", "",'K3'!A5)</f>
-        <v/>
-      </c>
-      <c r="B5" s="25" t="str">
+        <v>Jakob Lundby</v>
+      </c>
+      <c r="B5" s="25">
         <f>IF('K3'!A5="", "",'K3'!E5)</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="C5" s="37" t="str">
         <f>IF('K3'!A5="", "",'K3'!F5)</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="D5" s="35"/>
       <c r="E5" s="25"/>
@@ -7760,15 +7811,15 @@
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="str">
         <f>IF('K3'!A6="", "",'K3'!A6)</f>
-        <v/>
-      </c>
-      <c r="B6" s="25" t="str">
+        <v>Anders Alme Eng</v>
+      </c>
+      <c r="B6" s="25">
         <f>IF('K3'!A6="", "",'K3'!E6)</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="C6" s="37" t="str">
         <f>IF('K3'!A6="", "",'K3'!F6)</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="D6" s="35"/>
       <c r="E6" s="25"/>
@@ -7784,15 +7835,15 @@
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="str">
         <f>IF('K3'!A7="", "",'K3'!A7)</f>
-        <v/>
-      </c>
-      <c r="B7" s="25" t="str">
+        <v>Vegard Thon</v>
+      </c>
+      <c r="B7" s="25">
         <f>IF('K3'!A7="", "",'K3'!E7)</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="C7" s="37" t="str">
         <f>IF('K3'!A7="", "",'K3'!F7)</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="D7" s="35"/>
       <c r="E7" s="25"/>
@@ -7808,15 +7859,15 @@
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="str">
         <f>IF('K3'!A8="", "",'K3'!A8)</f>
-        <v/>
-      </c>
-      <c r="B8" s="25" t="str">
+        <v>Christian Thon Christensen</v>
+      </c>
+      <c r="B8" s="25">
         <f>IF('K3'!A8="", "",'K3'!E8)</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="C8" s="37" t="str">
         <f>IF('K3'!A8="", "",'K3'!F8)</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="D8" s="35"/>
       <c r="E8" s="25"/>
@@ -7832,15 +7883,15 @@
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="str">
         <f>IF('K3'!A9="", "",'K3'!A9)</f>
-        <v/>
-      </c>
-      <c r="B9" s="25" t="str">
+        <v>Per Ingvar Tollehaug</v>
+      </c>
+      <c r="B9" s="25">
         <f>IF('K3'!A9="", "",'K3'!E9)</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="C9" s="37" t="str">
         <f>IF('K3'!A9="", "",'K3'!F9)</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="D9" s="35"/>
       <c r="E9" s="25"/>
@@ -7856,15 +7907,15 @@
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="str">
         <f>IF('K3'!A10="", "",'K3'!A10)</f>
-        <v/>
-      </c>
-      <c r="B10" s="25" t="str">
+        <v>Hermann Byfuglien Ulsrud</v>
+      </c>
+      <c r="B10" s="25">
         <f>IF('K3'!A10="", "",'K3'!E10)</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="C10" s="37" t="str">
         <f>IF('K3'!A10="", "",'K3'!F10)</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="D10" s="35"/>
       <c r="E10" s="25"/>
@@ -7880,15 +7931,15 @@
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="9" t="str">
         <f>IF('K3'!A11="", "",'K3'!A11)</f>
-        <v/>
-      </c>
-      <c r="B11" s="25" t="str">
+        <v>Erland Andersen</v>
+      </c>
+      <c r="B11" s="25">
         <f>IF('K3'!A11="", "",'K3'!E11)</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="C11" s="37" t="str">
         <f>IF('K3'!A11="", "",'K3'!F11)</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="D11" s="35"/>
       <c r="E11" s="25"/>
@@ -10105,13 +10156,13 @@
   <sheetPr codeName="Sheet12" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:M103"/>
   <sheetViews>
-    <sheetView zoomScale="185" zoomScaleNormal="185" zoomScalePageLayoutView="185" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="185" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="15"/>
+    <col min="1" max="1" width="31.83203125" style="15" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.5" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.6640625" style="1" customWidth="1"/>
     <col min="4" max="13" width="8.83203125" style="1"/>
@@ -10173,15 +10224,15 @@
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="39" t="str">
         <f>IF('K3'!A4="", "",'K3'!A4)</f>
-        <v/>
-      </c>
-      <c r="B4" s="36" t="str">
+        <v>Brage Sømoen</v>
+      </c>
+      <c r="B4" s="36">
         <f>IF('K3'!A4="", "",'K3'!H4)</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="C4" s="37" t="str">
         <f>IF('K3'!A4="", "",'K3'!I4)</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="D4" s="11"/>
       <c r="E4" s="25"/>
@@ -10197,15 +10248,15 @@
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="39" t="str">
         <f>IF('K3'!A5="", "",'K3'!A5)</f>
-        <v/>
-      </c>
-      <c r="B5" s="36" t="str">
+        <v>Jakob Lundby</v>
+      </c>
+      <c r="B5" s="36">
         <f>IF('K3'!A5="", "",'K3'!H5)</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="C5" s="37" t="str">
         <f>IF('K3'!A5="", "",'K3'!I5)</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="D5" s="11"/>
       <c r="E5" s="25"/>
@@ -10221,15 +10272,15 @@
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="39" t="str">
         <f>IF('K3'!A6="", "",'K3'!A6)</f>
-        <v/>
-      </c>
-      <c r="B6" s="36" t="str">
+        <v>Anders Alme Eng</v>
+      </c>
+      <c r="B6" s="36">
         <f>IF('K3'!A6="", "",'K3'!H6)</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="C6" s="37" t="str">
         <f>IF('K3'!A6="", "",'K3'!I6)</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="D6" s="11"/>
       <c r="E6" s="25"/>
@@ -10245,15 +10296,15 @@
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="39" t="str">
         <f>IF('K3'!A7="", "",'K3'!A7)</f>
-        <v/>
-      </c>
-      <c r="B7" s="36" t="str">
+        <v>Vegard Thon</v>
+      </c>
+      <c r="B7" s="36">
         <f>IF('K3'!A7="", "",'K3'!H7)</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="C7" s="37" t="str">
         <f>IF('K3'!A7="", "",'K3'!I7)</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="D7" s="11"/>
       <c r="E7" s="25"/>
@@ -10269,15 +10320,15 @@
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="39" t="str">
         <f>IF('K3'!A8="", "",'K3'!A8)</f>
-        <v/>
-      </c>
-      <c r="B8" s="36" t="str">
+        <v>Christian Thon Christensen</v>
+      </c>
+      <c r="B8" s="36">
         <f>IF('K3'!A8="", "",'K3'!H8)</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="C8" s="37" t="str">
         <f>IF('K3'!A8="", "",'K3'!I8)</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="D8" s="11"/>
       <c r="E8" s="25"/>
@@ -10293,15 +10344,15 @@
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="39" t="str">
         <f>IF('K3'!A9="", "",'K3'!A9)</f>
-        <v/>
-      </c>
-      <c r="B9" s="36" t="str">
+        <v>Per Ingvar Tollehaug</v>
+      </c>
+      <c r="B9" s="36">
         <f>IF('K3'!A9="", "",'K3'!H9)</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="C9" s="37" t="str">
         <f>IF('K3'!A9="", "",'K3'!I9)</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="D9" s="11"/>
       <c r="E9" s="25"/>
@@ -10317,15 +10368,15 @@
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="39" t="str">
         <f>IF('K3'!A10="", "",'K3'!A10)</f>
-        <v/>
-      </c>
-      <c r="B10" s="36" t="str">
+        <v>Hermann Byfuglien Ulsrud</v>
+      </c>
+      <c r="B10" s="36">
         <f>IF('K3'!A10="", "",'K3'!H10)</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="C10" s="37" t="str">
         <f>IF('K3'!A10="", "",'K3'!I10)</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="D10" s="11"/>
       <c r="E10" s="25"/>
@@ -10341,15 +10392,15 @@
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="39" t="str">
         <f>IF('K3'!A11="", "",'K3'!A11)</f>
-        <v/>
-      </c>
-      <c r="B11" s="36" t="str">
+        <v>Erland Andersen</v>
+      </c>
+      <c r="B11" s="36">
         <f>IF('K3'!A11="", "",'K3'!H11)</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="C11" s="37" t="str">
         <f>IF('K3'!A11="", "",'K3'!I11)</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="D11" s="11"/>
       <c r="E11" s="25"/>
@@ -12564,12 +12615,13 @@
   <sheetPr codeName="Sheet13" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:S304"/>
   <sheetViews>
-    <sheetView zoomScale="174" zoomScaleNormal="174" zoomScalePageLayoutView="174" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="174" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="22.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="0" style="14" hidden="1" customWidth="1"/>
     <col min="3" max="3" width="8.83203125" style="14"/>
     <col min="4" max="5" width="8.83203125" style="15"/>
@@ -12685,7 +12737,7 @@
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="str">
         <f>IF('K3'!A7="", "",'K3'!A7)</f>
-        <v/>
+        <v>Vegard Thon</v>
       </c>
       <c r="B4" s="19" t="str">
         <f>IF('K3'!B7="", "",'K3'!B7)</f>
@@ -12697,11 +12749,11 @@
       </c>
       <c r="D4" s="23" t="str">
         <f>IF(A4="","",IFERROR(VLOOKUP(E4,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="E4" s="23" t="str">
         <f t="shared" ref="E4:E67" si="1">IF(A4="","",IFERROR(RANK(C4,C:C,1),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="F4" s="19" t="str">
         <f>IF('K3'!E7="", "", 'K3'!E7)</f>
@@ -12713,11 +12765,11 @@
       </c>
       <c r="H4" s="23" t="str">
         <f>IF(A4="","",IFERROR(VLOOKUP(I4,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="I4" s="23" t="str">
         <f t="shared" ref="I4:I67" si="3">IF(A4="","",IFERROR(RANK(G4,G:G,1),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="J4" s="19" t="str">
         <f>IF('K3'!H7="", "", 'K3'!H7)</f>
@@ -12729,11 +12781,11 @@
       </c>
       <c r="L4" s="23" t="str">
         <f>IF(A4="","",IFERROR(VLOOKUP(M4,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="M4" s="23" t="str">
         <f t="shared" ref="M4:M67" si="5">IF(A4="","",IFERROR(RANK(K4,K:K,1),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="N4" s="27" t="str">
         <f>IF('K3'!K7="", "", 'K3'!K7)</f>
@@ -12745,17 +12797,17 @@
       </c>
       <c r="P4" s="22" t="str">
         <f>IF(A4="", "",IFERROR(IF(D4+H4+L4=0,"",D4+H4+L4),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="Q4" s="23" t="str">
         <f t="shared" ref="Q4:Q67" si="7">IF(A4="","", IFERROR(RANK(P4,P:P,0),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="15" t="str">
         <f>IF('K3'!A6="", "",'K3'!A6)</f>
-        <v/>
+        <v>Anders Alme Eng</v>
       </c>
       <c r="B5" s="19" t="str">
         <f>IF('K3'!B6="", "",'K3'!B6)</f>
@@ -12767,11 +12819,11 @@
       </c>
       <c r="D5" s="23" t="str">
         <f>IF(A5="","",IFERROR(VLOOKUP(E5,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="E5" s="23" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="F5" s="19" t="str">
         <f>IF('K3'!E6="", "", 'K3'!E6)</f>
@@ -12783,11 +12835,11 @@
       </c>
       <c r="H5" s="23" t="str">
         <f>IF(A5="","",IFERROR(VLOOKUP(I5,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="I5" s="23" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="J5" s="19" t="str">
         <f>IF('K3'!H6="", "", 'K3'!H6)</f>
@@ -12799,11 +12851,11 @@
       </c>
       <c r="L5" s="23" t="str">
         <f>IF(A5="","",IFERROR(VLOOKUP(M5,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="M5" s="23" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="N5" s="27" t="str">
         <f>IF('K3'!K6="", "", 'K3'!K6)</f>
@@ -12815,11 +12867,11 @@
       </c>
       <c r="P5" s="23" t="str">
         <f t="shared" ref="P5:P68" si="8">IF(A5="", "",IFERROR(IF(D5+H5+L5=0,"",D5+H5+L5),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="Q5" s="23" t="str">
         <f t="shared" si="7"/>
-        <v/>
+        <v>-</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
@@ -12895,7 +12947,7 @@
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="15" t="str">
         <f>IF('K1'!A4="", "",'K1'!A4)</f>
-        <v/>
+        <v>Magnus Moslett Evensen</v>
       </c>
       <c r="B7" s="19" t="str">
         <f>IF('K1'!B4="", "",'K1'!B4)</f>
@@ -12907,11 +12959,11 @@
       </c>
       <c r="D7" s="23" t="str">
         <f>IF(A7="","",IFERROR(VLOOKUP(E7,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="E7" s="23" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="F7" s="19" t="str">
         <f>IF('K1'!E4="", "", 'K1'!E4)</f>
@@ -12923,11 +12975,11 @@
       </c>
       <c r="H7" s="23" t="str">
         <f>IF(A7="","",IFERROR(VLOOKUP(I7,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="I7" s="23" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="J7" s="19" t="str">
         <f>IF('K1'!H4="", "", 'K1'!H4)</f>
@@ -12939,11 +12991,11 @@
       </c>
       <c r="L7" s="23" t="str">
         <f>IF(A7="","",IFERROR(VLOOKUP(M7,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="M7" s="23" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="N7" s="27" t="str">
         <f>IF('K1'!K4="", "", 'K1'!K4)</f>
@@ -12955,11 +13007,11 @@
       </c>
       <c r="P7" s="23" t="str">
         <f t="shared" si="8"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="Q7" s="23" t="str">
         <f t="shared" si="7"/>
-        <v/>
+        <v>-</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
@@ -19685,7 +19737,7 @@
     <row r="104" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A104" s="15" t="str">
         <f>IF('K3'!A4="", "",'K3'!A4)</f>
-        <v/>
+        <v>Brage Sømoen</v>
       </c>
       <c r="B104" s="19" t="str">
         <f>IF('K3'!B4="", "",'K3'!B4)</f>
@@ -19697,11 +19749,11 @@
       </c>
       <c r="D104" s="23" t="str">
         <f>IF(A104="","",IFERROR(VLOOKUP(E104,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="E104" s="23" t="str">
         <f t="shared" si="10"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="F104" s="19" t="str">
         <f>IF('K3'!E4="", "", 'K3'!E4)</f>
@@ -19713,11 +19765,11 @@
       </c>
       <c r="H104" s="23" t="str">
         <f>IF(A104="","",IFERROR(VLOOKUP(I104,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="I104" s="23" t="str">
         <f t="shared" si="12"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="J104" s="19" t="str">
         <f>IF('K3'!H4="", "", 'K3'!H4)</f>
@@ -19729,11 +19781,11 @@
       </c>
       <c r="L104" s="23" t="str">
         <f>IF(A104="","",IFERROR(VLOOKUP(M104,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="M104" s="23" t="str">
         <f t="shared" si="14"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="N104" s="27" t="str">
         <f>IF('K3'!K4="", "", 'K3'!K4)</f>
@@ -19745,17 +19797,17 @@
       </c>
       <c r="P104" s="23" t="str">
         <f t="shared" si="17"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="Q104" s="23" t="str">
         <f t="shared" si="16"/>
-        <v/>
+        <v>-</v>
       </c>
     </row>
     <row r="105" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A105" s="15" t="str">
         <f>IF('K2'!A4="", "",'K2'!A4)</f>
-        <v/>
+        <v>Eskil Engdal</v>
       </c>
       <c r="B105" s="19" t="str">
         <f>IF('K2'!B4="", "",'K2'!B4)</f>
@@ -19767,11 +19819,11 @@
       </c>
       <c r="D105" s="23" t="str">
         <f>IF(A105="","",IFERROR(VLOOKUP(E105,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="E105" s="23" t="str">
         <f t="shared" si="10"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="F105" s="19" t="str">
         <f>IF('K2'!E4="", "", 'K2'!E4)</f>
@@ -19783,11 +19835,11 @@
       </c>
       <c r="H105" s="23" t="str">
         <f>IF(A105="","",IFERROR(VLOOKUP(I105,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="I105" s="23" t="str">
         <f t="shared" si="12"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="J105" s="19" t="str">
         <f>IF('K2'!H4="", "", 'K2'!H4)</f>
@@ -19799,11 +19851,11 @@
       </c>
       <c r="L105" s="23" t="str">
         <f>IF(A105="","",IFERROR(VLOOKUP(M105,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="M105" s="23" t="str">
         <f t="shared" si="14"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="N105" s="27" t="str">
         <f>IF('K2'!K4="", "", 'K2'!K4)</f>
@@ -19815,17 +19867,17 @@
       </c>
       <c r="P105" s="23" t="str">
         <f t="shared" si="17"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="Q105" s="23" t="str">
         <f t="shared" si="16"/>
-        <v/>
+        <v>-</v>
       </c>
     </row>
     <row r="106" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A106" s="15" t="str">
         <f>IF('K1'!A5="", "",'K1'!A5)</f>
-        <v/>
+        <v>Jonatan Heimdal Korshavn</v>
       </c>
       <c r="B106" s="19" t="str">
         <f>IF('K1'!B5="", "",'K1'!B5)</f>
@@ -19837,11 +19889,11 @@
       </c>
       <c r="D106" s="23" t="str">
         <f>IF(A106="","",IFERROR(VLOOKUP(E106,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="E106" s="23" t="str">
         <f t="shared" si="10"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="F106" s="19" t="str">
         <f>IF('K1'!E5="", "", 'K1'!E5)</f>
@@ -19853,11 +19905,11 @@
       </c>
       <c r="H106" s="23" t="str">
         <f>IF(A106="","",IFERROR(VLOOKUP(I106,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="I106" s="23" t="str">
         <f t="shared" si="12"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="J106" s="19" t="str">
         <f>IF('K1'!H5="", "", 'K1'!H5)</f>
@@ -19869,11 +19921,11 @@
       </c>
       <c r="L106" s="23" t="str">
         <f>IF(A106="","",IFERROR(VLOOKUP(M106,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="M106" s="23" t="str">
         <f t="shared" si="14"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="N106" s="27" t="str">
         <f>IF('K1'!K5="", "", 'K1'!K5)</f>
@@ -19885,11 +19937,11 @@
       </c>
       <c r="P106" s="23" t="str">
         <f t="shared" si="17"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="Q106" s="23" t="str">
         <f t="shared" si="16"/>
-        <v/>
+        <v>-</v>
       </c>
     </row>
     <row r="107" spans="1:17" x14ac:dyDescent="0.2">
@@ -26685,7 +26737,7 @@
     <row r="204" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A204" s="15" t="str">
         <f>IF('K2'!A5="", "",'K2'!A5)</f>
-        <v/>
+        <v>Tobias Gigstad Bergene</v>
       </c>
       <c r="B204" s="19" t="str">
         <f>IF('K2'!B5="", "",'K2'!B5)</f>
@@ -26697,11 +26749,11 @@
       </c>
       <c r="D204" s="23" t="str">
         <f>IF(A204="","",IFERROR(VLOOKUP(E204,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="E204" s="23" t="str">
         <f t="shared" si="28"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="F204" s="19" t="str">
         <f>IF('K2'!E5="", "", 'K2'!E5)</f>
@@ -26713,11 +26765,11 @@
       </c>
       <c r="H204" s="23" t="str">
         <f>IF(A204="","",IFERROR(VLOOKUP(I204,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="I204" s="23" t="str">
         <f t="shared" si="30"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="J204" s="19" t="str">
         <f>IF('K2'!H5="", "", 'K2'!H5)</f>
@@ -26729,11 +26781,11 @@
       </c>
       <c r="L204" s="23" t="str">
         <f>IF(A204="","",IFERROR(VLOOKUP(M204,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="M204" s="23" t="str">
         <f t="shared" si="32"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="N204" s="27" t="str">
         <f>IF('K2'!K5="", "", 'K2'!K5)</f>
@@ -26745,17 +26797,17 @@
       </c>
       <c r="P204" s="23" t="str">
         <f t="shared" si="35"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="Q204" s="23" t="str">
         <f t="shared" si="34"/>
-        <v/>
+        <v>-</v>
       </c>
     </row>
     <row r="205" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A205" s="15" t="str">
         <f>IF('K1'!A7="", "",'K1'!A7)</f>
-        <v/>
+        <v>Marius Granvold</v>
       </c>
       <c r="B205" s="19" t="str">
         <f>IF('K1'!B7="", "",'K1'!B7)</f>
@@ -26767,11 +26819,11 @@
       </c>
       <c r="D205" s="23" t="str">
         <f>IF(A205="","",IFERROR(VLOOKUP(E205,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="E205" s="23" t="str">
         <f t="shared" si="28"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="F205" s="19" t="str">
         <f>IF('K1'!E7="", "", 'K1'!E7)</f>
@@ -26783,11 +26835,11 @@
       </c>
       <c r="H205" s="23" t="str">
         <f>IF(A205="","",IFERROR(VLOOKUP(I205,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="I205" s="23" t="str">
         <f t="shared" si="30"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="J205" s="19" t="str">
         <f>IF('K1'!H7="", "", 'K1'!H7)</f>
@@ -26799,11 +26851,11 @@
       </c>
       <c r="L205" s="23" t="str">
         <f>IF(A205="","",IFERROR(VLOOKUP(M205,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="M205" s="23" t="str">
         <f t="shared" si="32"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="N205" s="27" t="str">
         <f>IF('K1'!K7="", "", 'K1'!K7)</f>
@@ -26815,17 +26867,17 @@
       </c>
       <c r="P205" s="23" t="str">
         <f t="shared" si="35"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="Q205" s="23" t="str">
         <f t="shared" si="34"/>
-        <v/>
+        <v>-</v>
       </c>
     </row>
     <row r="206" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A206" s="15" t="str">
         <f>IF('K1'!A6="", "",'K1'!A6)</f>
-        <v/>
+        <v>Martin Jørstad Ringli</v>
       </c>
       <c r="B206" s="19" t="str">
         <f>IF('K1'!B6="", "",'K1'!B6)</f>
@@ -26837,11 +26889,11 @@
       </c>
       <c r="D206" s="23" t="str">
         <f>IF(A206="","",IFERROR(VLOOKUP(E206,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="E206" s="23" t="str">
         <f t="shared" si="28"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="F206" s="19" t="str">
         <f>IF('K1'!E6="", "", 'K1'!E6)</f>
@@ -26853,11 +26905,11 @@
       </c>
       <c r="H206" s="23" t="str">
         <f>IF(A206="","",IFERROR(VLOOKUP(I206,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="I206" s="23" t="str">
         <f t="shared" si="30"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="J206" s="19" t="str">
         <f>IF('K1'!H6="", "", 'K1'!H6)</f>
@@ -26869,11 +26921,11 @@
       </c>
       <c r="L206" s="23" t="str">
         <f>IF(A206="","",IFERROR(VLOOKUP(M206,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="M206" s="23" t="str">
         <f t="shared" si="32"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="N206" s="27" t="str">
         <f>IF('K1'!K6="", "", 'K1'!K6)</f>
@@ -26885,17 +26937,17 @@
       </c>
       <c r="P206" s="23" t="str">
         <f t="shared" si="35"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="Q206" s="23" t="str">
         <f t="shared" si="34"/>
-        <v/>
+        <v>-</v>
       </c>
     </row>
     <row r="207" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A207" s="15" t="str">
         <f>IF('K3'!A5="", "",'K3'!A5)</f>
-        <v/>
+        <v>Jakob Lundby</v>
       </c>
       <c r="B207" s="19" t="str">
         <f>IF('K3'!B5="", "",'K3'!B5)</f>
@@ -26907,11 +26959,11 @@
       </c>
       <c r="D207" s="23" t="str">
         <f>IF(A207="","",IFERROR(VLOOKUP(E207,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="E207" s="23" t="str">
         <f t="shared" si="28"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="F207" s="19" t="str">
         <f>IF('K3'!E5="", "", 'K3'!E5)</f>
@@ -26923,11 +26975,11 @@
       </c>
       <c r="H207" s="23" t="str">
         <f>IF(A207="","",IFERROR(VLOOKUP(I207,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="I207" s="23" t="str">
         <f t="shared" si="30"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="J207" s="19" t="str">
         <f>IF('K3'!H5="", "", 'K3'!H5)</f>
@@ -26939,11 +26991,11 @@
       </c>
       <c r="L207" s="23" t="str">
         <f>IF(A207="","",IFERROR(VLOOKUP(M207,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="M207" s="23" t="str">
         <f t="shared" si="32"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="N207" s="27" t="str">
         <f>IF('K3'!K5="", "", 'K3'!K5)</f>
@@ -26955,17 +27007,17 @@
       </c>
       <c r="P207" s="23" t="str">
         <f t="shared" si="35"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="Q207" s="23" t="str">
         <f t="shared" si="34"/>
-        <v/>
+        <v>-</v>
       </c>
     </row>
     <row r="208" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A208" s="15" t="str">
         <f>IF('K3'!A8="", "",'K3'!A8)</f>
-        <v/>
+        <v>Christian Thon Christensen</v>
       </c>
       <c r="B208" s="19" t="str">
         <f>IF('K3'!B8="", "",'K3'!B8)</f>
@@ -26977,11 +27029,11 @@
       </c>
       <c r="D208" s="23" t="str">
         <f>IF(A208="","",IFERROR(VLOOKUP(E208,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="E208" s="23" t="str">
         <f t="shared" ref="E208:E268" si="37">IF(A208="","",IFERROR(RANK(C208,C:C,1),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="F208" s="19" t="str">
         <f>IF('K3'!E8="", "", 'K3'!E8)</f>
@@ -26993,11 +27045,11 @@
       </c>
       <c r="H208" s="23" t="str">
         <f>IF(A208="","",IFERROR(VLOOKUP(I208,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="I208" s="23" t="str">
         <f t="shared" ref="I208:I260" si="39">IF(A208="","",IFERROR(RANK(G208,G:G,1),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="J208" s="19" t="str">
         <f>IF('K3'!H8="", "", 'K3'!H8)</f>
@@ -27009,11 +27061,11 @@
       </c>
       <c r="L208" s="23" t="str">
         <f>IF(A208="","",IFERROR(VLOOKUP(M208,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="M208" s="23" t="str">
         <f t="shared" ref="M208:M260" si="41">IF(A208="","",IFERROR(RANK(K208,K:K,1),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="N208" s="27" t="str">
         <f>IF('K3'!K8="", "", 'K3'!K8)</f>
@@ -27025,17 +27077,17 @@
       </c>
       <c r="P208" s="23" t="str">
         <f t="shared" si="35"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="Q208" s="23" t="str">
         <f t="shared" ref="Q208:Q260" si="43">IF(A208="","", IFERROR(RANK(P208,P:P,0),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
     </row>
     <row r="209" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A209" s="15" t="str">
         <f>IF('K3'!A9="", "",'K3'!A9)</f>
-        <v/>
+        <v>Per Ingvar Tollehaug</v>
       </c>
       <c r="B209" s="19" t="str">
         <f>IF('K3'!B9="", "",'K3'!B9)</f>
@@ -27047,11 +27099,11 @@
       </c>
       <c r="D209" s="23" t="str">
         <f>IF(A209="","",IFERROR(VLOOKUP(E209,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="E209" s="23" t="str">
         <f t="shared" si="37"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="F209" s="19" t="str">
         <f>IF('K3'!E9="", "", 'K3'!E9)</f>
@@ -27063,11 +27115,11 @@
       </c>
       <c r="H209" s="23" t="str">
         <f>IF(A209="","",IFERROR(VLOOKUP(I209,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="I209" s="23" t="str">
         <f t="shared" si="39"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="J209" s="19" t="str">
         <f>IF('K3'!H9="", "", 'K3'!H9)</f>
@@ -27079,11 +27131,11 @@
       </c>
       <c r="L209" s="23" t="str">
         <f>IF(A209="","",IFERROR(VLOOKUP(M209,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="M209" s="23" t="str">
         <f t="shared" si="41"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="N209" s="27" t="str">
         <f>IF('K3'!K9="", "", 'K3'!K9)</f>
@@ -27095,17 +27147,17 @@
       </c>
       <c r="P209" s="23" t="str">
         <f t="shared" si="35"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="Q209" s="23" t="str">
         <f t="shared" si="43"/>
-        <v/>
+        <v>-</v>
       </c>
     </row>
     <row r="210" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A210" s="15" t="str">
         <f>IF('K3'!A10="", "",'K3'!A10)</f>
-        <v/>
+        <v>Hermann Byfuglien Ulsrud</v>
       </c>
       <c r="B210" s="19" t="str">
         <f>IF('K3'!B10="", "",'K3'!B10)</f>
@@ -27117,11 +27169,11 @@
       </c>
       <c r="D210" s="23" t="str">
         <f>IF(A210="","",IFERROR(VLOOKUP(E210,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="E210" s="23" t="str">
         <f t="shared" si="37"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="F210" s="19" t="str">
         <f>IF('K3'!E10="", "", 'K3'!E10)</f>
@@ -27133,11 +27185,11 @@
       </c>
       <c r="H210" s="23" t="str">
         <f>IF(A210="","",IFERROR(VLOOKUP(I210,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="I210" s="23" t="str">
         <f t="shared" si="39"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="J210" s="19" t="str">
         <f>IF('K3'!H10="", "", 'K3'!H10)</f>
@@ -27149,11 +27201,11 @@
       </c>
       <c r="L210" s="23" t="str">
         <f>IF(A210="","",IFERROR(VLOOKUP(M210,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="M210" s="23" t="str">
         <f t="shared" si="41"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="N210" s="27" t="str">
         <f>IF('K3'!K10="", "", 'K3'!K10)</f>
@@ -27165,17 +27217,17 @@
       </c>
       <c r="P210" s="23" t="str">
         <f t="shared" si="35"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="Q210" s="23" t="str">
         <f t="shared" si="43"/>
-        <v/>
+        <v>-</v>
       </c>
     </row>
     <row r="211" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A211" s="15" t="str">
         <f>IF('K3'!A11="", "",'K3'!A11)</f>
-        <v/>
+        <v>Erland Andersen</v>
       </c>
       <c r="B211" s="19" t="str">
         <f>IF('K3'!B11="", "",'K3'!B11)</f>
@@ -27187,11 +27239,11 @@
       </c>
       <c r="D211" s="23" t="str">
         <f>IF(A211="","",IFERROR(VLOOKUP(E211,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="E211" s="23" t="str">
         <f t="shared" si="37"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="F211" s="19" t="str">
         <f>IF('K3'!E11="", "", 'K3'!E11)</f>
@@ -27203,11 +27255,11 @@
       </c>
       <c r="H211" s="23" t="str">
         <f>IF(A211="","",IFERROR(VLOOKUP(I211,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="I211" s="23" t="str">
         <f t="shared" si="39"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="J211" s="19" t="str">
         <f>IF('K3'!H11="", "", 'K3'!H11)</f>
@@ -27219,11 +27271,11 @@
       </c>
       <c r="L211" s="23" t="str">
         <f>IF(A211="","",IFERROR(VLOOKUP(M211,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="M211" s="23" t="str">
         <f t="shared" si="41"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="N211" s="27" t="str">
         <f>IF('K3'!K11="", "", 'K3'!K11)</f>
@@ -27235,11 +27287,11 @@
       </c>
       <c r="P211" s="23" t="str">
         <f t="shared" si="35"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="Q211" s="23" t="str">
         <f t="shared" si="43"/>
-        <v/>
+        <v>-</v>
       </c>
     </row>
     <row r="212" spans="1:17" x14ac:dyDescent="0.2">
@@ -33711,13 +33763,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M303"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="185" zoomScaleNormal="185" zoomScalePageLayoutView="185" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="185" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="15"/>
+    <col min="1" max="1" width="37.33203125" style="15" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.5" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27.5" style="1" customWidth="1"/>
     <col min="4" max="13" width="8.83203125" style="1"/>
@@ -33779,15 +33831,15 @@
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="39" t="str">
         <f>IF(D1D2D3!A5="", "",D1D2D3!A5)</f>
-        <v/>
+        <v>Anders Alme Eng</v>
       </c>
       <c r="B4" s="41" t="str">
         <f>IF(D1D2D3!A5="", "",D1D2D3!P5)</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="C4" s="37" t="str">
         <f>IF(D1D2D3!A5="", "",D1D2D3!Q5)</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="D4" s="11"/>
       <c r="E4" s="25"/>
@@ -33803,15 +33855,15 @@
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="39" t="str">
         <f>IF(D1D2D3!A4="", "",D1D2D3!A4)</f>
-        <v/>
+        <v>Vegard Thon</v>
       </c>
       <c r="B5" s="41" t="str">
         <f>IF(D1D2D3!A4="", "",D1D2D3!P4)</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="C5" s="37" t="str">
         <f>IF(D1D2D3!A4="", "",D1D2D3!Q4)</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="D5" s="11"/>
       <c r="E5" s="25"/>
@@ -33827,15 +33879,15 @@
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="39" t="str">
         <f>IF(D1D2D3!A7="", "",D1D2D3!A7)</f>
-        <v/>
+        <v>Magnus Moslett Evensen</v>
       </c>
       <c r="B6" s="41" t="str">
         <f>IF(D1D2D3!A7="", "",D1D2D3!P7)</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="C6" s="37" t="str">
         <f>IF(D1D2D3!A7="", "",D1D2D3!Q7)</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="D6" s="11"/>
       <c r="E6" s="25"/>
@@ -36160,43 +36212,43 @@
     <row r="104" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A104" s="39" t="str">
         <f>IF(D1D2D3!A104="", "",D1D2D3!A104)</f>
-        <v/>
+        <v>Brage Sømoen</v>
       </c>
       <c r="B104" s="41" t="str">
         <f>IF(D1D2D3!A104="", "",D1D2D3!P104)</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="C104" s="37" t="str">
         <f>IF(D1D2D3!A104="", "",D1D2D3!Q104)</f>
-        <v/>
+        <v>-</v>
       </c>
     </row>
     <row r="105" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A105" s="39" t="str">
         <f>IF(D1D2D3!A105="", "",D1D2D3!A105)</f>
-        <v/>
+        <v>Eskil Engdal</v>
       </c>
       <c r="B105" s="41" t="str">
         <f>IF(D1D2D3!A105="", "",D1D2D3!P105)</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="C105" s="37" t="str">
         <f>IF(D1D2D3!A105="", "",D1D2D3!Q105)</f>
-        <v/>
+        <v>-</v>
       </c>
     </row>
     <row r="106" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A106" s="39" t="str">
         <f>IF(D1D2D3!A106="", "",D1D2D3!A106)</f>
-        <v/>
+        <v>Jonatan Heimdal Korshavn</v>
       </c>
       <c r="B106" s="41" t="str">
         <f>IF(D1D2D3!A106="", "",D1D2D3!P106)</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="C106" s="37" t="str">
         <f>IF(D1D2D3!A106="", "",D1D2D3!Q106)</f>
-        <v/>
+        <v>-</v>
       </c>
     </row>
     <row r="107" spans="1:13" x14ac:dyDescent="0.2">
@@ -37560,99 +37612,99 @@
     <row r="204" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A204" s="39" t="str">
         <f>IF(D1D2D3!A205="", "",D1D2D3!A205)</f>
-        <v/>
+        <v>Marius Granvold</v>
       </c>
       <c r="B204" s="41" t="str">
         <f>IF(D1D2D3!A205="", "",D1D2D3!P205)</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="C204" s="37" t="str">
         <f>IF(D1D2D3!A205="", "",D1D2D3!Q205)</f>
-        <v/>
+        <v>-</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A205" s="39" t="str">
         <f>IF(D1D2D3!A206="", "",D1D2D3!A206)</f>
-        <v/>
+        <v>Martin Jørstad Ringli</v>
       </c>
       <c r="B205" s="41" t="str">
         <f>IF(D1D2D3!A206="", "",D1D2D3!P206)</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="C205" s="37" t="str">
         <f>IF(D1D2D3!A206="", "",D1D2D3!Q206)</f>
-        <v/>
+        <v>-</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A206" s="39" t="str">
         <f>IF(D1D2D3!A207="", "",D1D2D3!A207)</f>
-        <v/>
+        <v>Jakob Lundby</v>
       </c>
       <c r="B206" s="41" t="str">
         <f>IF(D1D2D3!A207="", "",D1D2D3!P207)</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="C206" s="37" t="str">
         <f>IF(D1D2D3!A207="", "",D1D2D3!Q207)</f>
-        <v/>
+        <v>-</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A207" s="39" t="str">
         <f>IF(D1D2D3!A208="", "",D1D2D3!A208)</f>
-        <v/>
+        <v>Christian Thon Christensen</v>
       </c>
       <c r="B207" s="41" t="str">
         <f>IF(D1D2D3!A208="", "",D1D2D3!P208)</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="C207" s="37" t="str">
         <f>IF(D1D2D3!A208="", "",D1D2D3!Q208)</f>
-        <v/>
+        <v>-</v>
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A208" s="39" t="str">
         <f>IF(D1D2D3!A209="", "",D1D2D3!A209)</f>
-        <v/>
+        <v>Per Ingvar Tollehaug</v>
       </c>
       <c r="B208" s="41" t="str">
         <f>IF(D1D2D3!A209="", "",D1D2D3!P209)</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="C208" s="37" t="str">
         <f>IF(D1D2D3!A209="", "",D1D2D3!Q209)</f>
-        <v/>
+        <v>-</v>
       </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A209" s="39" t="str">
         <f>IF(D1D2D3!A210="", "",D1D2D3!A210)</f>
-        <v/>
+        <v>Hermann Byfuglien Ulsrud</v>
       </c>
       <c r="B209" s="41" t="str">
         <f>IF(D1D2D3!A210="", "",D1D2D3!P210)</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="C209" s="37" t="str">
         <f>IF(D1D2D3!A210="", "",D1D2D3!Q210)</f>
-        <v/>
+        <v>-</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A210" s="39" t="str">
         <f>IF(D1D2D3!A211="", "",D1D2D3!A211)</f>
-        <v/>
+        <v>Erland Andersen</v>
       </c>
       <c r="B210" s="41" t="str">
         <f>IF(D1D2D3!A211="", "",D1D2D3!P211)</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="C210" s="37" t="str">
         <f>IF(D1D2D3!A211="", "",D1D2D3!Q211)</f>
-        <v/>
+        <v>-</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.2">
@@ -38946,15 +38998,15 @@
     <row r="303" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A303" s="39" t="str">
         <f>IF(D1D2D3!A204="", "",D1D2D3!A204)</f>
-        <v/>
+        <v>Tobias Gigstad Bergene</v>
       </c>
       <c r="B303" s="41" t="str">
         <f>IF(D1D2D3!A204="", "",D1D2D3!P204)</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="C303" s="37" t="str">
         <f>IF(D1D2D3!A204="", "",D1D2D3!Q204)</f>
-        <v/>
+        <v>-</v>
       </c>
     </row>
   </sheetData>
@@ -38974,7 +39026,7 @@
   <sheetPr codeName="Sheet14" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:B133"/>
   <sheetViews>
-    <sheetView zoomScale="154" zoomScaleNormal="154" zoomScalePageLayoutView="154" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="154" workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
@@ -39750,13 +39802,13 @@
   <sheetPr codeName="Sheet2" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:M104"/>
   <sheetViews>
-    <sheetView zoomScale="185" zoomScaleNormal="185" zoomScalePageLayoutView="185" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="185" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="15"/>
+    <col min="1" max="1" width="23.6640625" style="15" customWidth="1"/>
     <col min="2" max="2" width="11.5" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="13" width="8.83203125" style="1"/>
     <col min="14" max="16384" width="8.83203125" style="15"/>
@@ -39843,33 +39895,35 @@
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" s="9"/>
+      <c r="A4" s="9" t="s">
+        <v>41</v>
+      </c>
       <c r="B4" s="25"/>
       <c r="C4" s="10" t="str">
         <f>IF(A4="","",IFERROR(RANK(B4,$B$4:$B$300,1),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="D4" s="11" t="str">
         <f>IF(A4="","", IFERROR(VLOOKUP(C4,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="E4" s="25"/>
       <c r="F4" s="10" t="str">
         <f>IF(A4="", "", IFERROR(RANK(E4,$E$4:$E$300,1),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="G4" s="11" t="str">
         <f>IF(A4="","",IFERROR(VLOOKUP(F4,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="H4" s="25"/>
       <c r="I4" s="10" t="str">
         <f>IF(A4="","",IFERROR(RANK(H4,$H$4:$H$300,1),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="J4" s="12" t="str">
         <f>IF(A4="","",IFERROR(VLOOKUP(I4,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="K4" s="26" t="str">
         <f>IF(A4="","",IFERROR(IF(B4+E4+H4=0,"",B4+E4+H4), "-"))</f>
@@ -39877,41 +39931,43 @@
       </c>
       <c r="L4" s="10" t="str">
         <f>IF(A4="","",IFERROR(RANK(M4,$M$4:$M$300,0),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="M4" s="12" t="str">
         <f>IF(A4="","",IFERROR(IF(D4+G4+J4=0,"0",D4+G4+J4),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="9"/>
+      <c r="A5" s="9" t="s">
+        <v>42</v>
+      </c>
       <c r="B5" s="25"/>
       <c r="C5" s="10" t="str">
         <f t="shared" ref="C5:C68" si="0">IF(A5="","",IFERROR(RANK(B5,$B$4:$B$300,1),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="D5" s="11" t="str">
         <f>IF(A5="","", IFERROR(VLOOKUP(C5,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="E5" s="25"/>
       <c r="F5" s="10" t="str">
         <f t="shared" ref="F5:F68" si="1">IF(A5="", "", IFERROR(RANK(E5,$E$4:$E$300,1),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="G5" s="11" t="str">
         <f>IF(A5="","",IFERROR(VLOOKUP(F5,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="H5" s="25"/>
       <c r="I5" s="10" t="str">
         <f t="shared" ref="I5:I68" si="2">IF(A5="","",IFERROR(RANK(H5,$H$4:$H$300,1),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="J5" s="12" t="str">
         <f>IF(A5="","",IFERROR(VLOOKUP(I5,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="K5" s="26" t="str">
         <f t="shared" ref="K5:K68" si="3">IF(A5="","",IFERROR(IF(B5+E5+H5=0,"",B5+E5+H5), "-"))</f>
@@ -39919,11 +39975,11 @@
       </c>
       <c r="L5" s="10" t="str">
         <f t="shared" ref="L5:L68" si="4">IF(A5="","",IFERROR(RANK(M5,$M$4:$M$300,0),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="M5" s="12" t="str">
         <f t="shared" ref="M5:M68" si="5">IF(A5="","",IFERROR(IF(D5+G5+J5=0,"0",D5+G5+J5),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
@@ -44063,13 +44119,13 @@
   <sheetPr codeName="Sheet3" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:M104"/>
   <sheetViews>
-    <sheetView zoomScale="185" zoomScaleNormal="185" zoomScalePageLayoutView="185" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="185" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="15"/>
+    <col min="1" max="1" width="25.5" style="15" customWidth="1"/>
     <col min="2" max="2" width="11.5" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="13" width="8.83203125" style="1"/>
     <col min="14" max="16384" width="8.83203125" style="15"/>
@@ -44156,33 +44212,35 @@
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" s="9"/>
+      <c r="A4" s="9" t="s">
+        <v>43</v>
+      </c>
       <c r="B4" s="25"/>
       <c r="C4" s="10" t="str">
         <f>IF(A4="","",IFERROR(RANK(B4,$B$4:$B$300,1),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="D4" s="11" t="str">
         <f>IF(A4="","", IFERROR(VLOOKUP(C4,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="E4" s="25"/>
       <c r="F4" s="10" t="str">
         <f>IF(A4="", "", IFERROR(RANK(E4,$E$4:$E$300,1),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="G4" s="11" t="str">
         <f>IF(A4="","",IFERROR(VLOOKUP(F4,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="H4" s="25"/>
       <c r="I4" s="10" t="str">
         <f>IF(A4="","",IFERROR(RANK(H4,$H$4:$H$300,1),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="J4" s="12" t="str">
         <f>IF(A4="","",IFERROR(VLOOKUP(I4,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="K4" s="26" t="str">
         <f>IF(A4="","",IFERROR(IF(B4+E4+H4=0,"",B4+E4+H4), "-"))</f>
@@ -44190,41 +44248,43 @@
       </c>
       <c r="L4" s="10" t="str">
         <f>IF(A4="","",IFERROR(RANK(M4,$M$4:$M$300,0),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="M4" s="12" t="str">
         <f>IF(A4="","",IFERROR(IF(D4+G4+J4=0,"0",D4+G4+J4),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="9"/>
+      <c r="A5" s="9" t="s">
+        <v>44</v>
+      </c>
       <c r="B5" s="25"/>
       <c r="C5" s="10" t="str">
         <f t="shared" ref="C5:C68" si="0">IF(A5="","",IFERROR(RANK(B5,$B$4:$B$300,1),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="D5" s="11" t="str">
         <f>IF(A5="","", IFERROR(VLOOKUP(C5,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="E5" s="25"/>
       <c r="F5" s="10" t="str">
         <f t="shared" ref="F5:F68" si="1">IF(A5="", "", IFERROR(RANK(E5,$E$4:$E$300,1),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="G5" s="11" t="str">
         <f>IF(A5="","",IFERROR(VLOOKUP(F5,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="H5" s="25"/>
       <c r="I5" s="10" t="str">
         <f t="shared" ref="I5:I68" si="2">IF(A5="","",IFERROR(RANK(H5,$H$4:$H$300,1),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="J5" s="12" t="str">
         <f>IF(A5="","",IFERROR(VLOOKUP(I5,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="K5" s="26" t="str">
         <f t="shared" ref="K5:K68" si="3">IF(A5="","",IFERROR(IF(B5+E5+H5=0,"",B5+E5+H5), "-"))</f>
@@ -44232,41 +44292,43 @@
       </c>
       <c r="L5" s="10" t="str">
         <f t="shared" ref="L5:L68" si="4">IF(A5="","",IFERROR(RANK(M5,$M$4:$M$300,0),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="M5" s="12" t="str">
         <f t="shared" ref="M5:M68" si="5">IF(A5="","",IFERROR(IF(D5+G5+J5=0,"0",D5+G5+J5),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="9"/>
+      <c r="A6" s="9" t="s">
+        <v>45</v>
+      </c>
       <c r="B6" s="25"/>
       <c r="C6" s="10" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="D6" s="11" t="str">
         <f>IF(A6="","", IFERROR(VLOOKUP(C6,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="E6" s="25"/>
       <c r="F6" s="10" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="G6" s="11" t="str">
         <f>IF(A6="","",IFERROR(VLOOKUP(F6,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="H6" s="25"/>
       <c r="I6" s="10" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="J6" s="12" t="str">
         <f>IF(A6="","",IFERROR(VLOOKUP(I6,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="K6" s="26" t="str">
         <f t="shared" si="3"/>
@@ -44274,41 +44336,43 @@
       </c>
       <c r="L6" s="10" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="M6" s="12" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>-</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="9"/>
+      <c r="A7" s="9" t="s">
+        <v>46</v>
+      </c>
       <c r="B7" s="25"/>
       <c r="C7" s="10" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="D7" s="11" t="str">
         <f>IF(A7="","", IFERROR(VLOOKUP(C7,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="E7" s="25"/>
       <c r="F7" s="10" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="G7" s="11" t="str">
         <f>IF(A7="","",IFERROR(VLOOKUP(F7,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="H7" s="25"/>
       <c r="I7" s="10" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="J7" s="12" t="str">
         <f>IF(A7="","",IFERROR(VLOOKUP(I7,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="K7" s="26" t="str">
         <f t="shared" si="3"/>
@@ -44316,41 +44380,43 @@
       </c>
       <c r="L7" s="10" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="M7" s="12" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>-</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="13"/>
+      <c r="A8" s="13" t="s">
+        <v>47</v>
+      </c>
       <c r="B8" s="25"/>
       <c r="C8" s="10" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="D8" s="11" t="str">
         <f>IF(A8="","", IFERROR(VLOOKUP(C8,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="E8" s="25"/>
       <c r="F8" s="10" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="G8" s="11" t="str">
         <f>IF(A8="","",IFERROR(VLOOKUP(F8,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="H8" s="25"/>
       <c r="I8" s="10" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="J8" s="12" t="str">
         <f>IF(A8="","",IFERROR(VLOOKUP(I8,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="K8" s="26" t="str">
         <f t="shared" si="3"/>
@@ -44358,41 +44424,43 @@
       </c>
       <c r="L8" s="10" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="M8" s="12" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>-</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A9" s="13"/>
+      <c r="A9" s="13" t="s">
+        <v>48</v>
+      </c>
       <c r="B9" s="25"/>
       <c r="C9" s="10" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="D9" s="11" t="str">
         <f>IF(A9="","", IFERROR(VLOOKUP(C9,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="E9" s="25"/>
       <c r="F9" s="10" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="G9" s="11" t="str">
         <f>IF(A9="","",IFERROR(VLOOKUP(F9,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="H9" s="25"/>
       <c r="I9" s="10" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="J9" s="12" t="str">
         <f>IF(A9="","",IFERROR(VLOOKUP(I9,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="K9" s="26" t="str">
         <f t="shared" si="3"/>
@@ -44400,41 +44468,43 @@
       </c>
       <c r="L9" s="10" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="M9" s="12" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>-</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A10" s="13"/>
+      <c r="A10" s="13" t="s">
+        <v>49</v>
+      </c>
       <c r="B10" s="25"/>
       <c r="C10" s="10" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="D10" s="11" t="str">
         <f>IF(A10="","", IFERROR(VLOOKUP(C10,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="E10" s="25"/>
       <c r="F10" s="10" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="G10" s="11" t="str">
         <f>IF(A10="","",IFERROR(VLOOKUP(F10,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="H10" s="25"/>
       <c r="I10" s="10" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="J10" s="12" t="str">
         <f>IF(A10="","",IFERROR(VLOOKUP(I10,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="K10" s="26" t="str">
         <f t="shared" si="3"/>
@@ -44442,41 +44512,43 @@
       </c>
       <c r="L10" s="10" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="M10" s="12" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>-</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="13"/>
+      <c r="A11" s="13" t="s">
+        <v>50</v>
+      </c>
       <c r="B11" s="25"/>
       <c r="C11" s="10" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="D11" s="11" t="str">
         <f>IF(A11="","", IFERROR(VLOOKUP(C11,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="E11" s="25"/>
       <c r="F11" s="10" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="G11" s="11" t="str">
         <f>IF(A11="","",IFERROR(VLOOKUP(F11,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="H11" s="25"/>
       <c r="I11" s="10" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="J11" s="12" t="str">
         <f>IF(A11="","",IFERROR(VLOOKUP(I11,Poengskala!$A$2:$B$134,2),"-"))</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="K11" s="26" t="str">
         <f t="shared" si="3"/>
@@ -44484,11 +44556,11 @@
       </c>
       <c r="L11" s="10" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>-</v>
       </c>
       <c r="M11" s="12" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>-</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
@@ -48376,13 +48448,13 @@
   <sheetPr codeName="Sheet4" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:M103"/>
   <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" zoomScalePageLayoutView="190" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="190" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="33"/>
+    <col min="1" max="1" width="31.83203125" style="33" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.5" style="40" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.6640625" style="40" customWidth="1"/>
     <col min="4" max="13" width="8.83203125" style="40"/>
@@ -48444,15 +48516,15 @@
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="39" t="str">
         <f>IF('K1'!A4="", "",'K1'!A4)</f>
-        <v/>
-      </c>
-      <c r="B4" s="36" t="str">
+        <v>Magnus Moslett Evensen</v>
+      </c>
+      <c r="B4" s="36">
         <f>IF('K1'!A4="", "",'K1'!B4)</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="C4" s="37" t="str">
         <f>IF('K1'!A4="", "",'K1'!C4)</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="D4" s="35"/>
       <c r="E4" s="36"/>
@@ -48468,15 +48540,15 @@
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="39" t="str">
         <f>IF('K1'!A5="", "",'K1'!A5)</f>
-        <v/>
-      </c>
-      <c r="B5" s="36" t="str">
+        <v>Jonatan Heimdal Korshavn</v>
+      </c>
+      <c r="B5" s="36">
         <f>IF('K1'!A5="", "",'K1'!B5)</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="C5" s="37" t="str">
         <f>IF('K1'!A5="", "",'K1'!C5)</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="D5" s="35"/>
       <c r="E5" s="36"/>
@@ -48492,15 +48564,15 @@
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="39" t="str">
         <f>IF('K1'!A6="", "",'K1'!A6)</f>
-        <v/>
-      </c>
-      <c r="B6" s="36" t="str">
+        <v>Martin Jørstad Ringli</v>
+      </c>
+      <c r="B6" s="36">
         <f>IF('K1'!A6="", "",'K1'!B6)</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="C6" s="37" t="str">
         <f>IF('K1'!A6="", "",'K1'!C6)</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="D6" s="35"/>
       <c r="E6" s="36"/>
@@ -48516,15 +48588,15 @@
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="39" t="str">
         <f>IF('K1'!A7="", "",'K1'!A7)</f>
-        <v/>
-      </c>
-      <c r="B7" s="36" t="str">
+        <v>Marius Granvold</v>
+      </c>
+      <c r="B7" s="36">
         <f>IF('K1'!A7="", "",'K1'!B7)</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="C7" s="37" t="str">
         <f>IF('K1'!A7="", "",'K1'!C7)</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="D7" s="35"/>
       <c r="E7" s="36"/>
@@ -50835,13 +50907,13 @@
   <sheetPr codeName="Sheet5" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:M103"/>
   <sheetViews>
-    <sheetView zoomScale="185" zoomScaleNormal="185" zoomScalePageLayoutView="185" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="185" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="15"/>
+    <col min="1" max="1" width="31.83203125" style="15" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.5" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.6640625" style="1" customWidth="1"/>
     <col min="4" max="13" width="8.83203125" style="1"/>
@@ -50903,15 +50975,15 @@
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="str">
         <f>IF('K1'!A4="", "",'K1'!A4)</f>
-        <v/>
-      </c>
-      <c r="B4" s="25" t="str">
+        <v>Magnus Moslett Evensen</v>
+      </c>
+      <c r="B4" s="25">
         <f>IF('K1'!A4="", "",'K1'!E4)</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="C4" s="37" t="str">
         <f>IF('K1'!A4="", "",'K1'!F4)</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="D4" s="35"/>
       <c r="E4" s="25"/>
@@ -50927,15 +50999,15 @@
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="str">
         <f>IF('K1'!A5="", "",'K1'!A5)</f>
-        <v/>
-      </c>
-      <c r="B5" s="25" t="str">
+        <v>Jonatan Heimdal Korshavn</v>
+      </c>
+      <c r="B5" s="25">
         <f>IF('K1'!A5="", "",'K1'!E5)</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="C5" s="37" t="str">
         <f>IF('K1'!A5="", "",'K1'!F5)</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="D5" s="35"/>
       <c r="E5" s="25"/>
@@ -50951,15 +51023,15 @@
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="str">
         <f>IF('K1'!A6="", "",'K1'!A6)</f>
-        <v/>
-      </c>
-      <c r="B6" s="25" t="str">
+        <v>Martin Jørstad Ringli</v>
+      </c>
+      <c r="B6" s="25">
         <f>IF('K1'!A6="", "",'K1'!E6)</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="C6" s="37" t="str">
         <f>IF('K1'!A6="", "",'K1'!F6)</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="D6" s="35"/>
       <c r="E6" s="25"/>
@@ -50975,15 +51047,15 @@
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="str">
         <f>IF('K1'!A7="", "",'K1'!A7)</f>
-        <v/>
-      </c>
-      <c r="B7" s="25" t="str">
+        <v>Marius Granvold</v>
+      </c>
+      <c r="B7" s="25">
         <f>IF('K1'!A7="", "",'K1'!E7)</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="C7" s="37" t="str">
         <f>IF('K1'!A7="", "",'K1'!F7)</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="D7" s="35"/>
       <c r="E7" s="25"/>
@@ -53296,13 +53368,13 @@
   <sheetPr codeName="Sheet6" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:M103"/>
   <sheetViews>
-    <sheetView zoomScale="185" zoomScaleNormal="185" zoomScalePageLayoutView="185" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="185" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="15"/>
+    <col min="1" max="1" width="31.83203125" style="15" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.5" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.6640625" style="1" customWidth="1"/>
     <col min="4" max="13" width="8.83203125" style="1"/>
@@ -53364,15 +53436,15 @@
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="39" t="str">
         <f>IF('K1'!A4="", "",'K1'!A4)</f>
-        <v/>
-      </c>
-      <c r="B4" s="36" t="str">
+        <v>Magnus Moslett Evensen</v>
+      </c>
+      <c r="B4" s="36">
         <f>IF('K1'!A4="", "",'K1'!H4)</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="C4" s="37" t="str">
         <f>IF('K1'!A4="", "",'K1'!I4)</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="D4" s="11"/>
       <c r="E4" s="25"/>
@@ -53388,15 +53460,15 @@
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="39" t="str">
         <f>IF('K1'!A5="", "",'K1'!A5)</f>
-        <v/>
-      </c>
-      <c r="B5" s="36" t="str">
+        <v>Jonatan Heimdal Korshavn</v>
+      </c>
+      <c r="B5" s="36">
         <f>IF('K1'!A5="", "",'K1'!H5)</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="C5" s="37" t="str">
         <f>IF('K1'!A5="", "",'K1'!I5)</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="D5" s="11"/>
       <c r="E5" s="25"/>
@@ -53412,15 +53484,15 @@
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="39" t="str">
         <f>IF('K1'!A6="", "",'K1'!A6)</f>
-        <v/>
-      </c>
-      <c r="B6" s="36" t="str">
+        <v>Martin Jørstad Ringli</v>
+      </c>
+      <c r="B6" s="36">
         <f>IF('K1'!A6="", "",'K1'!H6)</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="C6" s="37" t="str">
         <f>IF('K1'!A6="", "",'K1'!I6)</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="D6" s="11"/>
       <c r="E6" s="25"/>
@@ -53436,15 +53508,15 @@
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="39" t="str">
         <f>IF('K1'!A7="", "",'K1'!A7)</f>
-        <v/>
-      </c>
-      <c r="B7" s="36" t="str">
+        <v>Marius Granvold</v>
+      </c>
+      <c r="B7" s="36">
         <f>IF('K1'!A7="", "",'K1'!H7)</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="C7" s="37" t="str">
         <f>IF('K1'!A7="", "",'K1'!I7)</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="D7" s="11"/>
       <c r="E7" s="25"/>
@@ -55755,13 +55827,13 @@
   <sheetPr codeName="Sheet7" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:M103"/>
   <sheetViews>
-    <sheetView zoomScale="185" zoomScaleNormal="185" zoomScalePageLayoutView="185" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="185" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="33"/>
+    <col min="1" max="1" width="31.83203125" style="33" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.5" style="40" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.6640625" style="40" customWidth="1"/>
     <col min="4" max="13" width="8.83203125" style="40"/>
@@ -55823,15 +55895,15 @@
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="39" t="str">
         <f>IF('K2'!A4="", "",'K2'!A4)</f>
-        <v/>
-      </c>
-      <c r="B4" s="36" t="str">
+        <v>Eskil Engdal</v>
+      </c>
+      <c r="B4" s="36">
         <f>IF('K2'!A4="", "",'K2'!B4)</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="C4" s="37" t="str">
         <f>IF('K2'!A4="", "",'K2'!C4)</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="D4" s="35"/>
       <c r="E4" s="36"/>
@@ -55847,15 +55919,15 @@
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="39" t="str">
         <f>IF('K2'!A5="", "",'K2'!A5)</f>
-        <v/>
-      </c>
-      <c r="B5" s="36" t="str">
+        <v>Tobias Gigstad Bergene</v>
+      </c>
+      <c r="B5" s="36">
         <f>IF('K2'!A5="", "",'K2'!B5)</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="C5" s="37" t="str">
         <f>IF('K2'!A5="", "",'K2'!C5)</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="D5" s="35"/>
       <c r="E5" s="36"/>
@@ -58214,13 +58286,13 @@
   <sheetPr codeName="Sheet8" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:M103"/>
   <sheetViews>
-    <sheetView zoomScale="185" zoomScaleNormal="185" zoomScalePageLayoutView="185" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="185" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="15"/>
+    <col min="1" max="1" width="31.83203125" style="15" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.5" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.6640625" style="1" customWidth="1"/>
     <col min="4" max="13" width="8.83203125" style="1"/>
@@ -58282,15 +58354,15 @@
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="str">
         <f>IF('K2'!A4="", "",'K2'!A4)</f>
-        <v/>
-      </c>
-      <c r="B4" s="25" t="str">
+        <v>Eskil Engdal</v>
+      </c>
+      <c r="B4" s="25">
         <f>IF('K2'!A4="", "",'K2'!E4)</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="C4" s="37" t="str">
         <f>IF('K2'!A4="", "",'K2'!F4)</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="D4" s="35"/>
       <c r="E4" s="25"/>
@@ -58306,15 +58378,15 @@
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="str">
         <f>IF('K2'!A5="", "",'K2'!A5)</f>
-        <v/>
-      </c>
-      <c r="B5" s="25" t="str">
+        <v>Tobias Gigstad Bergene</v>
+      </c>
+      <c r="B5" s="25">
         <f>IF('K2'!A5="", "",'K2'!E5)</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="C5" s="37" t="str">
         <f>IF('K2'!A5="", "",'K2'!F5)</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="D5" s="35"/>
       <c r="E5" s="25"/>
@@ -60675,13 +60747,13 @@
   <sheetPr codeName="Sheet9" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:M103"/>
   <sheetViews>
-    <sheetView zoomScale="185" zoomScaleNormal="185" zoomScalePageLayoutView="185" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="185" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="15"/>
+    <col min="1" max="1" width="31.83203125" style="15" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.5" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.6640625" style="1" customWidth="1"/>
     <col min="4" max="13" width="8.83203125" style="1"/>
@@ -60743,15 +60815,15 @@
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="39" t="str">
         <f>IF('K2'!A4="", "",'K2'!A4)</f>
-        <v/>
-      </c>
-      <c r="B4" s="36" t="str">
+        <v>Eskil Engdal</v>
+      </c>
+      <c r="B4" s="36">
         <f>IF('K2'!A4="", "",'K2'!H4)</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="C4" s="37" t="str">
         <f>IF('K2'!A4="", "",'K2'!I4)</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="D4" s="11"/>
       <c r="E4" s="25"/>
@@ -60767,15 +60839,15 @@
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="39" t="str">
         <f>IF('K2'!A5="", "",'K2'!A5)</f>
-        <v/>
-      </c>
-      <c r="B5" s="36" t="str">
+        <v>Tobias Gigstad Bergene</v>
+      </c>
+      <c r="B5" s="36">
         <f>IF('K2'!A5="", "",'K2'!H5)</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="C5" s="37" t="str">
         <f>IF('K2'!A5="", "",'K2'!I5)</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="D5" s="11"/>
       <c r="E5" s="25"/>

</xml_diff>